<commit_message>
add fastest route stats to sheet for town 2
</commit_message>
<xml_diff>
--- a/ResourcesAndPlanning/Towns A-Star.xlsx
+++ b/ResourcesAndPlanning/Towns A-Star.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tom\Git\Hub\tomatport\m33193-ccc-self-driving-car\ResourcesAndPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F240DF-BA11-4E47-B11E-45A030F04C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B4EC4A1-4620-4D4C-93E4-E9F787E4518D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-480" yWindow="2610" windowWidth="28800" windowHeight="15345" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2520" yWindow="2400" windowWidth="28800" windowHeight="15345" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Town 1 Distance" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6158" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6166" uniqueCount="68">
   <si>
     <t>Calculate values for each node connected to start</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>fastest</t>
+  </si>
+  <si>
+    <t>optimal</t>
   </si>
 </sst>
 </file>
@@ -21873,8 +21879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D01440-B7EE-4A36-8CB9-B37F5724C4A3}">
   <dimension ref="A2:BC35"/>
   <sheetViews>
-    <sheetView topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="G35" sqref="E31:G35"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -25876,11 +25882,25 @@
         <v>35</v>
       </c>
     </row>
+    <row r="30" spans="1:55">
+      <c r="E30" t="s">
+        <v>67</v>
+      </c>
+      <c r="J30" t="s">
+        <v>66</v>
+      </c>
+    </row>
     <row r="31" spans="1:55">
       <c r="E31" t="s">
         <v>64</v>
       </c>
       <c r="G31" t="s">
+        <v>65</v>
+      </c>
+      <c r="J31" t="s">
+        <v>64</v>
+      </c>
+      <c r="L31" t="s">
         <v>65</v>
       </c>
     </row>
@@ -25896,8 +25916,19 @@
         <f>(F32/F35)*100</f>
         <v>44.840703756538282</v>
       </c>
+      <c r="J32" t="s">
+        <v>63</v>
+      </c>
+      <c r="K32">
+        <f>265+324+166</f>
+        <v>755</v>
+      </c>
+      <c r="L32">
+        <f>(K32/K35)*100</f>
+        <v>48.930654569021385</v>
+      </c>
     </row>
-    <row r="33" spans="5:7">
+    <row r="33" spans="5:12">
       <c r="E33" t="s">
         <v>61</v>
       </c>
@@ -25909,8 +25940,19 @@
         <f>(F33/F35)*100</f>
         <v>28.863528292914886</v>
       </c>
+      <c r="J33" t="s">
+        <v>61</v>
+      </c>
+      <c r="K33">
+        <f>347+282+159</f>
+        <v>788</v>
+      </c>
+      <c r="L33">
+        <f>(K33/K35)*100</f>
+        <v>51.069345430978608</v>
+      </c>
     </row>
-    <row r="34" spans="5:7">
+    <row r="34" spans="5:12">
       <c r="E34" t="s">
         <v>62</v>
       </c>
@@ -25922,14 +25964,31 @@
         <f>(F34/F35)*100</f>
         <v>26.295767950546839</v>
       </c>
+      <c r="J34" t="s">
+        <v>62</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <f>(K34/K35)*100</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="35" spans="5:7">
+    <row r="35" spans="5:12">
       <c r="E35" t="s">
         <v>60</v>
       </c>
       <c r="F35">
         <f>SUM(F32:F34)</f>
         <v>2103</v>
+      </c>
+      <c r="J35" t="s">
+        <v>60</v>
+      </c>
+      <c r="K35">
+        <f>SUM(K32:K34)</f>
+        <v>1543</v>
       </c>
     </row>
   </sheetData>
@@ -25951,7 +26010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9947A06-68E7-49A0-AEBD-B43F81758B60}">
   <dimension ref="A1:EI64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>

</xml_diff>